<commit_message>
BAJAJ-CD MIS Issue Resolve1
</commit_message>
<xml_diff>
--- a/media/BAJAJ-PL/MIS/FEB 22/BAJAJ-PL MIS.xlsx
+++ b/media/BAJAJ-PL/MIS/FEB 22/BAJAJ-PL MIS.xlsx
@@ -466,7 +466,7 @@
         <v>569158</v>
       </c>
       <c r="D2" t="n">
-        <v>5.343356211495236</v>
+        <v>5.34</v>
       </c>
     </row>
     <row r="3">
@@ -480,7 +480,7 @@
         <v>266418</v>
       </c>
       <c r="D3" t="n">
-        <v>1.523460729115686</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="4">
@@ -494,7 +494,7 @@
         <v>195378</v>
       </c>
       <c r="D4" t="n">
-        <v>1.846571912557905</v>
+        <v>1.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>